<commit_message>
time, size, xsec updated
</commit_message>
<xml_diff>
--- a/OfficialMC2012/RPVGluinoHeavyFlav/RPVGluinoHeavyFlav_clseitz.xlsx
+++ b/OfficialMC2012/RPVGluinoHeavyFlav/RPVGluinoHeavyFlav_clseitz.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="520" yWindow="0" windowWidth="25360" windowHeight="13920" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="RPVgluino_M_1000_8TeV_pythia6D6THC_113_223_cff.py" localSheetId="0">Sheet1!$B$2</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -57,77 +57,77 @@
     <t>M=200,  RPVgluino_M-200_113_223_TuneD6T_8Tev_pythia6</t>
   </si>
   <si>
-    <t>M=250,  RPVgluino_M-200_113_223_TuneD6T_8Tev_pythia6</t>
-  </si>
-  <si>
-    <t>M=300,  RPVgluino_M-200_113_223_TuneD6T_8Tev_pythia6</t>
-  </si>
-  <si>
-    <t>M=350,  RPVgluino_M-200_113_223_TuneD6T_8Tev_pythia6</t>
-  </si>
-  <si>
-    <t>M=400,  RPVgluino_M-200_113_223_TuneD6T_8Tev_pythia6</t>
-  </si>
-  <si>
-    <t>M=450,  RPVgluino_M-200_113_223_TuneD6T_8Tev_pythia6</t>
-  </si>
-  <si>
-    <t>M=500,  RPVgluino_M-200_113_223_TuneD6T_8Tev_pythia6</t>
-  </si>
-  <si>
-    <t>M=1000,  RPVgluino_M-200_113_223_TuneD6T_8Tev_pythia6</t>
-  </si>
-  <si>
-    <t>M=750,  RPVgluino_M-200_113_223_TuneD6T_8Tev_pythia6</t>
-  </si>
-  <si>
-    <t>M=1500,  RPVgluino_M-200_113_223_TuneD6T_8Tev_pythia6</t>
-  </si>
-  <si>
-    <t>M=1250,  RPVgluino_M-200_113_223_TuneD6T_8Tev_pythia6</t>
-  </si>
-  <si>
     <t>RPV gluinos -&gt; 2j + b, Requester Claudia Seitz</t>
   </si>
   <si>
-    <t>RPVgluino_M_1000_8TeV_pythia5DTHC_113_223_cff.py</t>
-  </si>
-  <si>
-    <t>RPVgluino_M_200_8TeV_pythia5DTHC_113_223_cff.py</t>
-  </si>
-  <si>
-    <t>RPVgluino_M_250_8TeV_pythia5DTHC_113_223_cff.py</t>
-  </si>
-  <si>
-    <t>RPVgluino_M_300_8TeV_pythia5DTHC_113_223_cff.py</t>
-  </si>
-  <si>
-    <t>RPVgluino_M_350_8TeV_pythia5DTHC_113_223_cff.py</t>
-  </si>
-  <si>
-    <t>RPVgluino_M_400_8TeV_pythia5DTHC_113_223_cff.py</t>
-  </si>
-  <si>
-    <t>RPVgluino_M_450_8TeV_pythia5DTHC_113_223_cff.py</t>
-  </si>
-  <si>
-    <t>RPVgluino_M_500_8TeV_pythia5DTHC_113_223_cff.py</t>
-  </si>
-  <si>
-    <t>RPVgluino_M_750_8TeV_pythia5DTHC_113_223_cff.py</t>
-  </si>
-  <si>
-    <t>RPVgluino_M_1250_8TeV_pythia5DTHC_113_223_cff.py</t>
-  </si>
-  <si>
-    <t>RPVgluino_M_1500_8TeV_pythia5DTHC_113_223_cff.py</t>
+    <t>RPVgluino_M_200_8TeV_pythia6D6THC_113_223_cff.py</t>
+  </si>
+  <si>
+    <t>RPVgluino_M_250_8TeV_pythia6D6THC_113_223_cff.py</t>
+  </si>
+  <si>
+    <t>RPVgluino_M_300_8TeV_pythia6D6THC_113_223_cff.py</t>
+  </si>
+  <si>
+    <t>RPVgluino_M_350_8TeV_pythia6D6THC_113_223_cff.py</t>
+  </si>
+  <si>
+    <t>RPVgluino_M_400_8TeV_pythia6D6THC_113_223_cff.py</t>
+  </si>
+  <si>
+    <t>RPVgluino_M_450_8TeV_pythia6D6THC_113_223_cff.py</t>
+  </si>
+  <si>
+    <t>RPVgluino_M_500_8TeV_pythia6D6THC_113_223_cff.py</t>
+  </si>
+  <si>
+    <t>RPVgluino_M_750_8TeV_pythia6D6THC_113_223_cff.py</t>
+  </si>
+  <si>
+    <t>RPVgluino_M_1000_8TeV_pythia6D6THC_113_223_cff.py</t>
+  </si>
+  <si>
+    <t>RPVgluino_M_1250_8TeV_pythia6D6THC_113_223_cff.py</t>
+  </si>
+  <si>
+    <t>RPVgluino_M_1500_8TeV_pythia6D6THC_113_223_cff.py</t>
+  </si>
+  <si>
+    <t>M=250,  RPVgluino_M-250_113_223_TuneD6T_8Tev_pythia6</t>
+  </si>
+  <si>
+    <t>M=300,  RPVgluino_M-300_113_223_TuneD6T_8Tev_pythia6</t>
+  </si>
+  <si>
+    <t>M=350,  RPVgluino_M-350_113_223_TuneD6T_8Tev_pythia6</t>
+  </si>
+  <si>
+    <t>M=400,  RPVgluino_M-400_113_223_TuneD6T_8Tev_pythia6</t>
+  </si>
+  <si>
+    <t>M=400,  RPVgluino_M-450_113_223_TuneD6T_8Tev_pythia6</t>
+  </si>
+  <si>
+    <t>M=500,  RPVgluino_M-500_113_223_TuneD6T_8Tev_pythia6</t>
+  </si>
+  <si>
+    <t>M=750,  RPVgluino_M-750_113_223_TuneD6T_8Tev_pythia6</t>
+  </si>
+  <si>
+    <t>M=1000,  RPVgluino_M-1000_113_223_TuneD6T_8Tev_pythia6</t>
+  </si>
+  <si>
+    <t>M=1250,  RPVgluino_M-1250_113_223_TuneD6T_8Tev_pythia6</t>
+  </si>
+  <si>
+    <t>M=1500,  RPVgluino_M-1500_113_223_TuneD6T_8Tev_pythia6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -162,8 +162,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -182,8 +187,14 @@
         <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDCE6F1"/>
+        <bgColor rgb="FFDCE6F1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -287,8 +298,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF95B3D7"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -309,8 +335,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -335,8 +363,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="20">
+  <cellStyles count="22">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -347,6 +378,7 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -356,43 +388,10 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="0"/>
-        <name val="Helvetica Neue"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -685,14 +684,14 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
         <name val="Helvetica Neue"/>
         <scheme val="none"/>
       </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
+          <fgColor rgb="FFDCE6F1"/>
+          <bgColor rgb="FFDCE6F1"/>
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -704,7 +703,7 @@
           <color auto="1"/>
         </right>
         <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
+          <color rgb="FF95B3D7"/>
         </top>
         <bottom style="thin">
           <color auto="1"/>
@@ -753,22 +752,56 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="0"/>
+        <name val="Helvetica Neue"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color auto="1"/>
         </left>
         <right style="thin">
           <color auto="1"/>
         </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -777,22 +810,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K12" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="10" tableBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K12" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9">
   <autoFilter ref="A1:K12"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="RPV gluinos -&gt; 2j + b, Requester Claudia Seitz" dataDxfId="9"/>
-    <tableColumn id="2" name="Name of generator fragment " dataDxfId="8"/>
-    <tableColumn id="3" name="EOS" dataDxfId="7"/>
-    <tableColumn id="4" name="events" dataDxfId="6"/>
-    <tableColumn id="5" name="Match. Eff." dataDxfId="5"/>
-    <tableColumn id="6" name="X-sec [pb]" dataDxfId="4"/>
-    <tableColumn id="7" name="Gen evts" dataDxfId="3"/>
+    <tableColumn id="1" name="RPV gluinos -&gt; 2j + b, Requester Claudia Seitz" dataDxfId="8"/>
+    <tableColumn id="2" name="Name of generator fragment " dataDxfId="7"/>
+    <tableColumn id="3" name="EOS" dataDxfId="6"/>
+    <tableColumn id="4" name="events" dataDxfId="5"/>
+    <tableColumn id="5" name="Match. Eff." dataDxfId="4"/>
+    <tableColumn id="6" name="X-sec [pb]" dataDxfId="3"/>
+    <tableColumn id="7" name="Gen evts" dataDxfId="2"/>
     <tableColumn id="8" name="CPUtime"/>
     <tableColumn id="9" name="size(B)"/>
-    <tableColumn id="10" name="CPU time/event [s]" dataDxfId="2">
+    <tableColumn id="10" name="CPU time/event [s]" dataDxfId="1">
       <calculatedColumnFormula>H2/G2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="size/event [kB]" dataDxfId="1">
+    <tableColumn id="11" name="size/event [kB]" dataDxfId="0">
       <calculatedColumnFormula>I2/G2*1/1024</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1125,13 +1158,13 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="57" customWidth="1"/>
-    <col min="2" max="2" width="51.83203125" customWidth="1"/>
+    <col min="1" max="1" width="60.1640625" customWidth="1"/>
+    <col min="2" max="2" width="55.33203125" customWidth="1"/>
     <col min="4" max="4" width="11.1640625" customWidth="1"/>
     <col min="5" max="5" width="15.6640625" customWidth="1"/>
     <col min="6" max="6" width="7" customWidth="1"/>
@@ -1144,7 +1177,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="18">
       <c r="A1" s="5" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
@@ -1181,8 +1214,8 @@
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>23</v>
+      <c r="B2" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1">
@@ -1214,10 +1247,10 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>13</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1">
@@ -1249,10 +1282,10 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>14</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1">
@@ -1284,10 +1317,10 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>15</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1">
@@ -1319,10 +1352,10 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1">
@@ -1354,10 +1387,10 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>17</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1">
@@ -1389,10 +1422,10 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>18</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1">
@@ -1424,10 +1457,10 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>19</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1">
@@ -1459,10 +1492,10 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>20</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1">
@@ -1494,10 +1527,10 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="1" t="s">
         <v>31</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>21</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1">
@@ -1529,10 +1562,10 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="1" t="s">
         <v>32</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>22</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1">
@@ -1604,7 +1637,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>